<commit_message>
a lot of updates to strain_comparison
</commit_message>
<xml_diff>
--- a/Allele.xlsx
+++ b/Allele.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="Allele"/>
   </sheets>
   <definedNames>
-    <definedName name="Allele">'Allele'!$A$1:$U$147</definedName>
+    <definedName name="Allele">'Allele'!$A$1:$U$151</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -343,7 +343,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U147"/>
+  <dimension ref="A1:U151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -2636,7 +2636,7 @@
       </c>
       <c r="F37" s="0" t="inlineStr">
         <is>
-          <t>∆me::cat-hpt</t>
+          <t>∆me::PgapD-cat-hpt</t>
         </is>
       </c>
       <c r="G37" s="0" t="b">
@@ -5522,7 +5522,7 @@
       </c>
       <c r="F109" s="0" t="inlineStr">
         <is>
-          <t>pSH007(PgapDH-adhE)</t>
+          <t>pSH007(PgapD-adhE)</t>
         </is>
       </c>
       <c r="G109" s="0" t="b">
@@ -5560,7 +5560,7 @@
       </c>
       <c r="F110" s="0" t="inlineStr">
         <is>
-          <t>∆pta::cat-hpt</t>
+          <t>∆pta::PgapD-cat-hpt</t>
         </is>
       </c>
       <c r="G110" s="0" t="b">
@@ -5682,16 +5682,21 @@
       </c>
       <c r="C112" s="0" t="inlineStr">
         <is>
-          <t>tscEtoh2</t>
+          <t>tscEtoh2int</t>
+        </is>
+      </c>
+      <c r="D112" s="0" t="inlineStr">
+        <is>
+          <t>ethanol</t>
         </is>
       </c>
       <c r="F112" s="0" t="inlineStr">
         <is>
-          <t>pSH64(P2638-nfnAB(Tsc)-adhA(Tsc))</t>
+          <t>P2638::pSH64(P2638-nfnAB(Tsc)-adhA(Tsc))</t>
         </is>
       </c>
       <c r="G112" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H112" s="0" t="inlineStr">
         <is>
@@ -5720,7 +5725,7 @@
       </c>
       <c r="N112" s="0" t="inlineStr">
         <is>
-          <t>nfnAB and adhA on a plasmid</t>
+          <t>pSH064 integrated in chromosome at Clo1313_2638 locus</t>
         </is>
       </c>
       <c r="T112" s="0" t="inlineStr">
@@ -6046,6 +6051,11 @@
           <t>tscEtoh3</t>
         </is>
       </c>
+      <c r="D121" s="0" t="inlineStr">
+        <is>
+          <t>ethanol</t>
+        </is>
+      </c>
       <c r="F121" s="0" t="inlineStr">
         <is>
           <t>P2638::adhA(Tsc)-nfnAB(Tsc)</t>
@@ -6079,6 +6089,11 @@
           <t>tscEtoh4</t>
         </is>
       </c>
+      <c r="D122" s="0" t="inlineStr">
+        <is>
+          <t>ethanol</t>
+        </is>
+      </c>
       <c r="F122" s="0" t="inlineStr">
         <is>
           <t>Ptsc0046-pforA(Tsc)-ferredoxin(Tsc)</t>
@@ -6300,6 +6315,11 @@
           <t>ppdk3</t>
         </is>
       </c>
+      <c r="D128" s="0" t="inlineStr">
+        <is>
+          <t>malate shunt</t>
+        </is>
+      </c>
       <c r="F128" s="0" t="inlineStr">
         <is>
           <t>ppdk::pZJ03</t>
@@ -6406,12 +6426,17 @@
       </c>
       <c r="C131" s="0" t="inlineStr">
         <is>
-          <t>tscEtoh5</t>
+          <t>tscEtoh5int</t>
+        </is>
+      </c>
+      <c r="D131" s="0" t="inlineStr">
+        <is>
+          <t>ethanol</t>
         </is>
       </c>
       <c r="F131" s="0" t="inlineStr">
         <is>
-          <t>pSH62(P2638-adhE(Tsc)-nfnAB(Tsc)-adhA(Tsc))</t>
+          <t>P2638::pSH62(P2638-adhE(Tsc)-nfnAB(Tsc)-adhA(Tsc))</t>
         </is>
       </c>
       <c r="G131" s="0" t="b">
@@ -6444,7 +6469,7 @@
       </c>
       <c r="N131" s="0" t="inlineStr">
         <is>
-          <t>Expression plasmid with T. sacch adhE-nfnAB-adhA</t>
+          <t>pSH062 integrated in chromosome at Clo1313_2638 locus</t>
         </is>
       </c>
       <c r="T131" s="0" t="inlineStr">
@@ -6477,7 +6502,7 @@
       </c>
       <c r="F132" s="0" t="inlineStr">
         <is>
-          <t>Δbcaat</t>
+          <t>ΔazlCD</t>
         </is>
       </c>
       <c r="G132" s="0" t="b">
@@ -6510,7 +6535,7 @@
       </c>
       <c r="N132" s="0" t="inlineStr">
         <is>
-          <t>Called in AG1326 and AG2069</t>
+          <t>Called in AG1326 and AG2069, also known as ilvT, bcaat, azlCD or brnEF</t>
         </is>
       </c>
       <c r="U132" s="0">
@@ -6528,7 +6553,7 @@
       </c>
       <c r="C133" s="0" t="inlineStr">
         <is>
-          <t>bcat1</t>
+          <t>ilvE1</t>
         </is>
       </c>
       <c r="D133" s="0" t="inlineStr">
@@ -6538,7 +6563,7 @@
       </c>
       <c r="F133" s="0" t="inlineStr">
         <is>
-          <t>Δbcat</t>
+          <t>ΔilvE</t>
         </is>
       </c>
       <c r="G133" s="0" t="b">
@@ -6571,7 +6596,7 @@
       </c>
       <c r="N133" s="0" t="inlineStr">
         <is>
-          <t>Called in AG1218, also known as ilvE</t>
+          <t>Called in AG1218, also known as ilvE and bcat</t>
         </is>
       </c>
       <c r="U133" s="0">
@@ -7380,6 +7405,204 @@
       </c>
       <c r="U147" s="0">
         <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="148">
+      <c r="A148" s="0">
+        <v>150</v>
+      </c>
+      <c r="B148" s="0" t="inlineStr">
+        <is>
+          <t>Clostridium thermocellum</t>
+        </is>
+      </c>
+      <c r="C148" s="0" t="inlineStr">
+        <is>
+          <t>ppdk4</t>
+        </is>
+      </c>
+      <c r="D148" s="0" t="inlineStr">
+        <is>
+          <t>malate shunt</t>
+        </is>
+      </c>
+      <c r="F148" s="0" t="inlineStr">
+        <is>
+          <t>Δppdk::PgapD-cat-hpt</t>
+        </is>
+      </c>
+      <c r="G148" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="H148" s="0" t="inlineStr">
+        <is>
+          <t>NC_017304.1</t>
+        </is>
+      </c>
+      <c r="I148" s="0" t="inlineStr">
+        <is>
+          <t>1105704</t>
+        </is>
+      </c>
+      <c r="J148" s="0" t="inlineStr">
+        <is>
+          <t>1107289</t>
+        </is>
+      </c>
+      <c r="K148" s="0" t="inlineStr">
+        <is>
+          <t>Insertion</t>
+        </is>
+      </c>
+      <c r="L148" s="0" t="inlineStr">
+        <is>
+          <t>pZJ03_mero_region</t>
+        </is>
+      </c>
+      <c r="N148" s="0" t="inlineStr">
+        <is>
+          <t>Partial deletion of ppdk using pZJ03, 355 bp removed</t>
+        </is>
+      </c>
+      <c r="U148" s="0">
+        <v>1585</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="149">
+      <c r="A149" s="0">
+        <v>151</v>
+      </c>
+      <c r="B149" s="0" t="inlineStr">
+        <is>
+          <t>Clostridium thermocellum</t>
+        </is>
+      </c>
+      <c r="C149" s="0" t="inlineStr">
+        <is>
+          <t>tscEtoh2</t>
+        </is>
+      </c>
+      <c r="D149" s="0" t="inlineStr">
+        <is>
+          <t>ethanol</t>
+        </is>
+      </c>
+      <c r="F149" s="0" t="inlineStr">
+        <is>
+          <t>pSH64(P2638-nfnAB(Tsc)-adhA(Tsc))</t>
+        </is>
+      </c>
+      <c r="G149" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="H149" s="0" t="inlineStr">
+        <is>
+          <t>pSH064</t>
+        </is>
+      </c>
+      <c r="N149" s="0" t="inlineStr">
+        <is>
+          <t>Expression plasmid with T. sacch nfnAB-adhA</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="150">
+      <c r="A150" s="0">
+        <v>152</v>
+      </c>
+      <c r="B150" s="0" t="inlineStr">
+        <is>
+          <t>Clostridium thermocellum</t>
+        </is>
+      </c>
+      <c r="C150" s="0" t="inlineStr">
+        <is>
+          <t>tscEtoh5</t>
+        </is>
+      </c>
+      <c r="D150" s="0" t="inlineStr">
+        <is>
+          <t>ethanol</t>
+        </is>
+      </c>
+      <c r="F150" s="0" t="inlineStr">
+        <is>
+          <t>pSH62(P2638-adhE(Tsc)-nfnAB(Tsc)-adhA(Tsc))</t>
+        </is>
+      </c>
+      <c r="G150" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="H150" s="0" t="inlineStr">
+        <is>
+          <t>pSH062</t>
+        </is>
+      </c>
+      <c r="N150" s="0" t="inlineStr">
+        <is>
+          <t>Expression plasmid with T. sacch adhE-nfnAB-adhA</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="151">
+      <c r="A151" s="0">
+        <v>153</v>
+      </c>
+      <c r="B151" s="0" t="inlineStr">
+        <is>
+          <t>Clostridium thermocellum</t>
+        </is>
+      </c>
+      <c r="C151" s="0" t="inlineStr">
+        <is>
+          <t>bcaat2</t>
+        </is>
+      </c>
+      <c r="D151" s="0" t="inlineStr">
+        <is>
+          <t>amino acid</t>
+        </is>
+      </c>
+      <c r="F151" s="0" t="inlineStr">
+        <is>
+          <t>ΔClo1313_0817-Clo1313_0826</t>
+        </is>
+      </c>
+      <c r="G151" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H151" s="0" t="inlineStr">
+        <is>
+          <t>NC_017304.1</t>
+        </is>
+      </c>
+      <c r="I151" s="0" t="inlineStr">
+        <is>
+          <t>941487</t>
+        </is>
+      </c>
+      <c r="J151" s="0" t="inlineStr">
+        <is>
+          <t>953492</t>
+        </is>
+      </c>
+      <c r="K151" s="0" t="inlineStr">
+        <is>
+          <t>Deletion</t>
+        </is>
+      </c>
+      <c r="M151" s="0" t="inlineStr">
+        <is>
+          <t>Clo1313_0817-Clo1313_0826</t>
+        </is>
+      </c>
+      <c r="N151" s="0" t="inlineStr">
+        <is>
+          <t>Spontaneous deletion of chromosomal region containing bcaat, probably due to recombination of flanking IS200 sequences</t>
+        </is>
+      </c>
+      <c r="U151" s="0">
+        <v>12005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>